<commit_message>
Fixed day plot. scatter misaligned now
</commit_message>
<xml_diff>
--- a/HRV trend test data.xlsx
+++ b/HRV trend test data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcte\Non OneDrive Docs\GitHub\HRVApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA60B7-BB89-4DCD-93BE-6A4A0173B6EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A81150-0DA2-4D51-B178-37F2CA86C33C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8486" yWindow="1946" windowWidth="23580" windowHeight="16603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5057" yWindow="1911" windowWidth="27009" windowHeight="16603" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -203,146 +203,164 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$52</c:f>
+              <c:f>Sheet1!$O$7:$O$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="36">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="37">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="38">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="39">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="40">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="41">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="42">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="43">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="44">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="45">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="46">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="47">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="48">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="49">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="50">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="51">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -350,10 +368,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$7:$P$52</c:f>
+              <c:f>Sheet1!$P$7:$P$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -491,6 +509,24 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,155 +899,170 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$R$7:$R$55</c:f>
+              <c:f>Sheet1!$R$7:$R$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="19">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="25">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="29">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="30">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="31">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="32">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="33">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="34">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="35">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="36">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="37">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="38">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="39">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="40">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="41">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="42">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="43">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="44">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="45">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="46">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="47">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="48">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="49">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="50">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="51">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="52">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="53">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1019,155 +1070,170 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$7:$S$55</c:f>
+              <c:f>Sheet1!$S$7:$S$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="19">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="25">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>33.666668000000001</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="29">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="31">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="32">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="33">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="34">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="35">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="36">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="37">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="38">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="39">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="40">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="41">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="42">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="43">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="44">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="45">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="46">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="47">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="48">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="50">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="51">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="53">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2939,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A13" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="AG62" sqref="AG62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3022,15 +3088,15 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>48</v>
+      <c r="B7" s="1">
+        <v>53</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <f>B7*$H$4+C7*$H$5</f>
-        <v>4150800</v>
+        <f t="shared" ref="D7:D12" si="0">B7*$H$4+C7*$H$5</f>
+        <v>4586400</v>
       </c>
       <c r="E7" cm="1">
         <f t="array" ref="E7">INDEX($L$7:$L$23,MOD(A7,17)+1,1)</f>
@@ -3041,14 +3107,14 @@
       </c>
       <c r="O7">
         <f>B7</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P7">
         <f>E7</f>
         <v>24</v>
       </c>
-      <c r="R7">
-        <v>48</v>
+      <c r="R7" s="1">
+        <v>53</v>
       </c>
       <c r="S7">
         <v>24</v>
@@ -3058,15 +3124,15 @@
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>46</v>
+      <c r="B8" s="1">
+        <v>52</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D52" si="0">B8*$H$4+C8*$H$5</f>
-        <v>3985200</v>
+        <f t="shared" si="0"/>
+        <v>4500000</v>
       </c>
       <c r="E8" cm="1">
         <f t="array" ref="E8">INDEX($L$7:$L$23,MOD(A8,17)+1,1)</f>
@@ -3076,33 +3142,33 @@
         <v>24</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8:O52" si="1">B8</f>
-        <v>46</v>
+        <f>B8</f>
+        <v>52</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P52" si="2">E8</f>
+        <f>E8</f>
         <v>26</v>
       </c>
-      <c r="R8">
-        <v>47</v>
+      <c r="R8" s="1">
+        <v>52</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9">
-        <v>46</v>
+      <c r="B9" s="1">
+        <v>51</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>3988800</v>
+        <v>4413600</v>
       </c>
       <c r="E9" cm="1">
         <f t="array" ref="E9">INDEX($L$7:$L$23,MOD(A9,17)+1,1)</f>
@@ -3112,33 +3178,33 @@
         <v>26</v>
       </c>
       <c r="O9">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f>B9</f>
+        <v>51</v>
       </c>
       <c r="P9">
-        <f t="shared" si="2"/>
+        <f>E9</f>
         <v>22</v>
       </c>
-      <c r="R9">
-        <v>46</v>
+      <c r="R9" s="1">
+        <v>51</v>
       </c>
       <c r="S9">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10">
-        <v>46</v>
+      <c r="B10" s="1">
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>3996000</v>
+        <v>4327200</v>
       </c>
       <c r="E10" cm="1">
         <f t="array" ref="E10">INDEX($L$7:$L$23,MOD(A10,17)+1,1)</f>
@@ -3148,33 +3214,33 @@
         <v>22</v>
       </c>
       <c r="O10">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f>B10</f>
+        <v>50</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
+        <f>E10</f>
         <v>30</v>
       </c>
-      <c r="R10">
-        <v>45</v>
+      <c r="R10" s="1">
+        <v>50</v>
       </c>
       <c r="S10">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11">
-        <v>45</v>
+      <c r="B11" s="1">
+        <v>49</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>3895200</v>
+        <v>4240800</v>
       </c>
       <c r="E11" cm="1">
         <f t="array" ref="E11">INDEX($L$7:$L$23,MOD(A11,17)+1,1)</f>
@@ -3184,33 +3250,33 @@
         <v>30</v>
       </c>
       <c r="O11">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <f>B11</f>
+        <v>49</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
+        <f>E11</f>
         <v>35</v>
       </c>
-      <c r="R11">
-        <v>44</v>
+      <c r="R11" s="1">
+        <v>49</v>
       </c>
       <c r="S11">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12">
-        <v>44</v>
+      <c r="B12" s="1">
+        <v>48</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>3812400</v>
+        <v>4154400</v>
       </c>
       <c r="E12" cm="1">
         <f t="array" ref="E12">INDEX($L$7:$L$23,MOD(A12,17)+1,1)</f>
@@ -3220,33 +3286,33 @@
         <v>35</v>
       </c>
       <c r="O12">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>B12</f>
+        <v>48</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f>E12</f>
         <v>38</v>
       </c>
-      <c r="R12">
-        <v>43</v>
+      <c r="R12" s="1">
+        <v>48</v>
       </c>
       <c r="S12">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13">
-        <v>43</v>
+      <c r="B13" s="1">
+        <v>47</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>3726000</v>
+        <f>B13*$H$4+C13*$H$5</f>
+        <v>4064400</v>
       </c>
       <c r="E13" cm="1">
         <f t="array" ref="E13">INDEX($L$7:$L$23,MOD(A13,17)+1,1)</f>
@@ -3256,18 +3322,18 @@
         <v>38</v>
       </c>
       <c r="O13">
-        <f t="shared" si="1"/>
+        <f>B13</f>
+        <v>47</v>
+      </c>
+      <c r="P13">
+        <f>E13</f>
         <v>43</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
       <c r="R13">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="S13">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
@@ -3275,14 +3341,14 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>3639600</v>
+        <f>B14*$H$4+C14*$H$5</f>
+        <v>3985200</v>
       </c>
       <c r="E14" cm="1">
         <f t="array" ref="E14">INDEX($L$7:$L$23,MOD(A14,17)+1,1)</f>
@@ -3292,18 +3358,18 @@
         <v>43</v>
       </c>
       <c r="O14">
-        <f t="shared" si="1"/>
+        <f>B14</f>
+        <v>46</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:P58" si="1">E14</f>
         <v>42</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
       <c r="R14">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="S14">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
@@ -3311,14 +3377,14 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>3553200</v>
+        <f>B15*$H$4+C15*$H$5</f>
+        <v>3988800</v>
       </c>
       <c r="E15" cm="1">
         <f t="array" ref="E15">INDEX($L$7:$L$23,MOD(A15,17)+1,1)</f>
@@ -3328,18 +3394,18 @@
         <v>42</v>
       </c>
       <c r="O15">
+        <f>B15</f>
+        <v>46</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="R15">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S15">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
@@ -3347,14 +3413,14 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>3466800</v>
+        <f>B16*$H$4+C16*$H$5</f>
+        <v>3996000</v>
       </c>
       <c r="E16" cm="1">
         <f t="array" ref="E16">INDEX($L$7:$L$23,MOD(A16,17)+1,1)</f>
@@ -3364,18 +3430,18 @@
         <v>39</v>
       </c>
       <c r="O16">
+        <f>B16</f>
+        <v>46</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="R16">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="S16">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
@@ -3383,14 +3449,14 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>3380400</v>
+        <f>B17*$H$4+C17*$H$5</f>
+        <v>3895200</v>
       </c>
       <c r="E17" cm="1">
         <f t="array" ref="E17">INDEX($L$7:$L$23,MOD(A17,17)+1,1)</f>
@@ -3400,18 +3466,18 @@
         <v>20</v>
       </c>
       <c r="O17">
+        <f>B17</f>
+        <v>45</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="R17">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="S17">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
@@ -3419,14 +3485,14 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>3294000</v>
+        <f>B18*$H$4+C18*$H$5</f>
+        <v>3812400</v>
       </c>
       <c r="E18" cm="1">
         <f t="array" ref="E18">INDEX($L$7:$L$23,MOD(A18,17)+1,1)</f>
@@ -3436,18 +3502,18 @@
         <v>17</v>
       </c>
       <c r="O18">
+        <f>B18</f>
+        <v>44</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R18">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="S18">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
@@ -3455,14 +3521,14 @@
         <v>13</v>
       </c>
       <c r="B19">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>3207600</v>
+        <f>B19*$H$4+C19*$H$5</f>
+        <v>3726000</v>
       </c>
       <c r="E19" cm="1">
         <f t="array" ref="E19">INDEX($L$7:$L$23,MOD(A19,17)+1,1)</f>
@@ -3472,18 +3538,18 @@
         <v>35</v>
       </c>
       <c r="O19">
+        <f>B19</f>
+        <v>43</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R19">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="S19">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
@@ -3491,14 +3557,14 @@
         <v>14</v>
       </c>
       <c r="B20">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>3121200</v>
+        <f>B20*$H$4+C20*$H$5</f>
+        <v>3639600</v>
       </c>
       <c r="E20" cm="1">
         <f t="array" ref="E20">INDEX($L$7:$L$23,MOD(A20,17)+1,1)</f>
@@ -3508,18 +3574,18 @@
         <v>23</v>
       </c>
       <c r="O20">
+        <f>B20</f>
+        <v>42</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R20">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="S20">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
@@ -3527,14 +3593,14 @@
         <v>15</v>
       </c>
       <c r="B21">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>3034800</v>
+        <f>B21*$H$4+C21*$H$5</f>
+        <v>3553200</v>
       </c>
       <c r="E21" cm="1">
         <f t="array" ref="E21">INDEX($L$7:$L$23,MOD(A21,17)+1,1)</f>
@@ -3544,18 +3610,18 @@
         <v>23</v>
       </c>
       <c r="O21">
+        <f>B21</f>
+        <v>41</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="R21">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="S21">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
@@ -3563,14 +3629,14 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>2948400</v>
+        <f>B22*$H$4+C22*$H$5</f>
+        <v>3466800</v>
       </c>
       <c r="E22" cm="1">
         <f t="array" ref="E22">INDEX($L$7:$L$23,MOD(A22,17)+1,1)</f>
@@ -3580,18 +3646,18 @@
         <v>25</v>
       </c>
       <c r="O22">
+        <f>B22</f>
+        <v>40</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="R22">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="S22">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
@@ -3599,14 +3665,14 @@
         <v>17</v>
       </c>
       <c r="B23">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>2862000</v>
+        <f>B23*$H$4+C23*$H$5</f>
+        <v>3380400</v>
       </c>
       <c r="E23" cm="1">
         <f t="array" ref="E23">INDEX($L$7:$L$23,MOD(A23,17)+1,1)</f>
@@ -3616,18 +3682,18 @@
         <v>26</v>
       </c>
       <c r="O23">
+        <f>B23</f>
+        <v>39</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="R23">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="S23">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
@@ -3635,14 +3701,14 @@
         <v>18</v>
       </c>
       <c r="B24">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>2775600</v>
+        <f>B24*$H$4+C24*$H$5</f>
+        <v>3294000</v>
       </c>
       <c r="E24" cm="1">
         <f t="array" ref="E24">INDEX($L$7:$L$23,MOD(A24,17)+1,1)</f>
@@ -3652,18 +3718,18 @@
         <v>27</v>
       </c>
       <c r="O24">
+        <f>B24</f>
+        <v>38</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="R24">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="S24">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
@@ -3671,32 +3737,32 @@
         <v>19</v>
       </c>
       <c r="B25">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>2689200</v>
+        <f>B25*$H$4+C25*$H$5</f>
+        <v>3207600</v>
       </c>
       <c r="E25" cm="1">
         <f t="array" ref="E25">INDEX($L$7:$L$23,MOD(A25,17)+1,1)</f>
         <v>26</v>
       </c>
       <c r="O25">
+        <f>B25</f>
+        <v>37</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="R25">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S25">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
@@ -3704,32 +3770,32 @@
         <v>20</v>
       </c>
       <c r="B26">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>2602800</v>
+        <f>B26*$H$4+C26*$H$5</f>
+        <v>3121200</v>
       </c>
       <c r="E26" cm="1">
         <f t="array" ref="E26">INDEX($L$7:$L$23,MOD(A26,17)+1,1)</f>
         <v>22</v>
       </c>
       <c r="O26">
+        <f>B26</f>
+        <v>36</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="R26">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="S26">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
@@ -3737,32 +3803,32 @@
         <v>21</v>
       </c>
       <c r="B27">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>2516400</v>
+        <f>B27*$H$4+C27*$H$5</f>
+        <v>3034800</v>
       </c>
       <c r="E27" cm="1">
         <f t="array" ref="E27">INDEX($L$7:$L$23,MOD(A27,17)+1,1)</f>
         <v>30</v>
       </c>
       <c r="O27">
+        <f>B27</f>
+        <v>35</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="R27">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="S27">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.4">
@@ -3770,32 +3836,32 @@
         <v>22</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
-        <v>2430000</v>
+        <f>B28*$H$4+C28*$H$5</f>
+        <v>2948400</v>
       </c>
       <c r="E28" cm="1">
         <f t="array" ref="E28">INDEX($L$7:$L$23,MOD(A28,17)+1,1)</f>
         <v>35</v>
       </c>
       <c r="O28">
+        <f>B28</f>
+        <v>34</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R28">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="S28">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
@@ -3803,32 +3869,32 @@
         <v>23</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>2343600</v>
+        <f>B29*$H$4+C29*$H$5</f>
+        <v>2862000</v>
       </c>
       <c r="E29" cm="1">
         <f t="array" ref="E29">INDEX($L$7:$L$23,MOD(A29,17)+1,1)</f>
         <v>38</v>
       </c>
       <c r="O29">
+        <f>B29</f>
+        <v>33</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="R29">
+        <v>31</v>
+      </c>
+      <c r="S29">
         <v>26</v>
-      </c>
-      <c r="S29">
-        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.4">
@@ -3836,32 +3902,32 @@
         <v>24</v>
       </c>
       <c r="B30">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
-        <v>2257200</v>
+        <f>B30*$H$4+C30*$H$5</f>
+        <v>2775600</v>
       </c>
       <c r="E30" cm="1">
         <f t="array" ref="E30">INDEX($L$7:$L$23,MOD(A30,17)+1,1)</f>
         <v>43</v>
       </c>
       <c r="O30">
+        <f>B30</f>
+        <v>32</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="R30">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="S30">
-        <v>33.666668000000001</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.4">
@@ -3869,32 +3935,32 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
-        <v>2170800</v>
+        <f>B31*$H$4+C31*$H$5</f>
+        <v>2689200</v>
       </c>
       <c r="E31" cm="1">
         <f t="array" ref="E31">INDEX($L$7:$L$23,MOD(A31,17)+1,1)</f>
         <v>42</v>
       </c>
       <c r="O31">
+        <f>B31</f>
+        <v>31</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="R31">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="S31">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.4">
@@ -3902,32 +3968,32 @@
         <v>26</v>
       </c>
       <c r="B32">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
-        <v>2170800</v>
+        <f>B32*$H$4+C32*$H$5</f>
+        <v>2602800</v>
       </c>
       <c r="E32" cm="1">
         <f t="array" ref="E32">INDEX($L$7:$L$23,MOD(A32,17)+1,1)</f>
         <v>39</v>
       </c>
       <c r="O32">
+        <f>B32</f>
+        <v>30</v>
+      </c>
+      <c r="P32">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="R32">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="S32">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.4">
@@ -3935,32 +4001,32 @@
         <v>27</v>
       </c>
       <c r="B33">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
-        <v>2170800</v>
+        <f>B33*$H$4+C33*$H$5</f>
+        <v>2516400</v>
       </c>
       <c r="E33" cm="1">
         <f t="array" ref="E33">INDEX($L$7:$L$23,MOD(A33,17)+1,1)</f>
         <v>20</v>
       </c>
       <c r="O33">
+        <f>B33</f>
+        <v>29</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="R33">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="S33">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.4">
@@ -3968,32 +4034,32 @@
         <v>28</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
-        <v>1911600</v>
+        <f>B34*$H$4+C34*$H$5</f>
+        <v>2430000</v>
       </c>
       <c r="E34" cm="1">
         <f t="array" ref="E34">INDEX($L$7:$L$23,MOD(A34,17)+1,1)</f>
         <v>17</v>
       </c>
       <c r="O34">
+        <f>B34</f>
+        <v>28</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="R34">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="S34">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.4">
@@ -4001,32 +4067,32 @@
         <v>29</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
-        <v>1825200</v>
+        <f>B35*$H$4+C35*$H$5</f>
+        <v>2343600</v>
       </c>
       <c r="E35" cm="1">
         <f t="array" ref="E35">INDEX($L$7:$L$23,MOD(A35,17)+1,1)</f>
         <v>35</v>
       </c>
       <c r="O35">
+        <f>B35</f>
+        <v>27</v>
+      </c>
+      <c r="P35">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R35">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="S35">
-        <v>23</v>
+        <v>33.666668000000001</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.4">
@@ -4034,32 +4100,32 @@
         <v>30</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
-        <v>1738800</v>
+        <f>B36*$H$4+C36*$H$5</f>
+        <v>2257200</v>
       </c>
       <c r="E36" cm="1">
         <f t="array" ref="E36">INDEX($L$7:$L$23,MOD(A36,17)+1,1)</f>
         <v>23</v>
       </c>
       <c r="O36">
+        <f>B36</f>
+        <v>26</v>
+      </c>
+      <c r="P36">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R36">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S36">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.4">
@@ -4067,32 +4133,32 @@
         <v>31</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
-        <v>1652400</v>
+        <f>B37*$H$4+C37*$H$5</f>
+        <v>2170800</v>
       </c>
       <c r="E37" cm="1">
         <f t="array" ref="E37">INDEX($L$7:$L$23,MOD(A37,17)+1,1)</f>
         <v>23</v>
       </c>
       <c r="O37">
+        <f>B37</f>
+        <v>25</v>
+      </c>
+      <c r="P37">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R37">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S37">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.4">
@@ -4100,32 +4166,32 @@
         <v>32</v>
       </c>
       <c r="B38">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
-        <v>1566000</v>
+        <f>B38*$H$4+C38*$H$5</f>
+        <v>2170800</v>
       </c>
       <c r="E38" cm="1">
         <f t="array" ref="E38">INDEX($L$7:$L$23,MOD(A38,17)+1,1)</f>
         <v>25</v>
       </c>
       <c r="O38">
+        <f>B38</f>
+        <v>25</v>
+      </c>
+      <c r="P38">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="R38">
+        <v>22</v>
+      </c>
+      <c r="S38">
         <v>17</v>
-      </c>
-      <c r="S38">
-        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.4">
@@ -4133,32 +4199,32 @@
         <v>33</v>
       </c>
       <c r="B39">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
-        <v>1479600</v>
+        <f>B39*$H$4+C39*$H$5</f>
+        <v>2170800</v>
       </c>
       <c r="E39" cm="1">
         <f t="array" ref="E39">INDEX($L$7:$L$23,MOD(A39,17)+1,1)</f>
         <v>26</v>
       </c>
       <c r="O39">
+        <f>B39</f>
+        <v>25</v>
+      </c>
+      <c r="P39">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="R39">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="S39">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.4">
@@ -4166,32 +4232,32 @@
         <v>34</v>
       </c>
       <c r="B40">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
-        <v>1393200</v>
+        <f>B40*$H$4+C40*$H$5</f>
+        <v>1911600</v>
       </c>
       <c r="E40" cm="1">
         <f t="array" ref="E40">INDEX($L$7:$L$23,MOD(A40,17)+1,1)</f>
         <v>19</v>
       </c>
       <c r="O40">
+        <f>B40</f>
+        <v>22</v>
+      </c>
+      <c r="P40">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="R40">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S40">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.4">
@@ -4199,32 +4265,32 @@
         <v>35</v>
       </c>
       <c r="B41">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41">
-        <f t="shared" si="0"/>
-        <v>1306800</v>
+        <f>B41*$H$4+C41*$H$5</f>
+        <v>1825200</v>
       </c>
       <c r="E41" cm="1">
         <f t="array" ref="E41">INDEX($L$7:$L$23,MOD(A41,17)+1,1)</f>
         <v>24</v>
       </c>
       <c r="O41">
+        <f>B41</f>
+        <v>21</v>
+      </c>
+      <c r="P41">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="P41">
-        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="R41">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="S41">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.4">
@@ -4232,32 +4298,32 @@
         <v>36</v>
       </c>
       <c r="B42">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42">
-        <f t="shared" si="0"/>
-        <v>1220400</v>
+        <f>B42*$H$4+C42*$H$5</f>
+        <v>1738800</v>
       </c>
       <c r="E42" cm="1">
         <f t="array" ref="E42">INDEX($L$7:$L$23,MOD(A42,17)+1,1)</f>
         <v>26</v>
       </c>
       <c r="O42">
+        <f>B42</f>
+        <v>20</v>
+      </c>
+      <c r="P42">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="R42">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="S42">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.4">
@@ -4265,32 +4331,32 @@
         <v>37</v>
       </c>
       <c r="B43">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43">
-        <f t="shared" si="0"/>
-        <v>1134000</v>
+        <f>B43*$H$4+C43*$H$5</f>
+        <v>1652400</v>
       </c>
       <c r="E43" cm="1">
         <f t="array" ref="E43">INDEX($L$7:$L$23,MOD(A43,17)+1,1)</f>
         <v>22</v>
       </c>
       <c r="O43">
+        <f>B43</f>
+        <v>19</v>
+      </c>
+      <c r="P43">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="R43">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="S43">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
@@ -4298,32 +4364,32 @@
         <v>38</v>
       </c>
       <c r="B44">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44">
-        <f t="shared" si="0"/>
-        <v>1047600</v>
+        <f>B44*$H$4+C44*$H$5</f>
+        <v>1566000</v>
       </c>
       <c r="E44" cm="1">
         <f t="array" ref="E44">INDEX($L$7:$L$23,MOD(A44,17)+1,1)</f>
         <v>30</v>
       </c>
       <c r="O44">
+        <f>B44</f>
+        <v>18</v>
+      </c>
+      <c r="P44">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="R44">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="S44">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.4">
@@ -4331,32 +4397,32 @@
         <v>39</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45">
-        <f t="shared" si="0"/>
-        <v>961200</v>
+        <f>B45*$H$4+C45*$H$5</f>
+        <v>1479600</v>
       </c>
       <c r="E45" cm="1">
         <f t="array" ref="E45">INDEX($L$7:$L$23,MOD(A45,17)+1,1)</f>
         <v>35</v>
       </c>
       <c r="O45">
+        <f>B45</f>
+        <v>17</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R45">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="S45">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.4">
@@ -4364,32 +4430,32 @@
         <v>40</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46">
-        <f t="shared" si="0"/>
-        <v>874800</v>
+        <f>B46*$H$4+C46*$H$5</f>
+        <v>1393200</v>
       </c>
       <c r="E46" cm="1">
         <f t="array" ref="E46">INDEX($L$7:$L$23,MOD(A46,17)+1,1)</f>
         <v>38</v>
       </c>
       <c r="O46">
+        <f>B46</f>
+        <v>16</v>
+      </c>
+      <c r="P46">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="R46">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="S46">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.4">
@@ -4397,32 +4463,32 @@
         <v>41</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47">
-        <f t="shared" si="0"/>
-        <v>788400</v>
+        <f>B47*$H$4+C47*$H$5</f>
+        <v>1306800</v>
       </c>
       <c r="E47" cm="1">
         <f t="array" ref="E47">INDEX($L$7:$L$23,MOD(A47,17)+1,1)</f>
         <v>43</v>
       </c>
       <c r="O47">
+        <f>B47</f>
+        <v>15</v>
+      </c>
+      <c r="P47">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="R47">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="S47">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.4">
@@ -4430,32 +4496,32 @@
         <v>42</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48">
-        <f t="shared" si="0"/>
-        <v>702000</v>
+        <f>B48*$H$4+C48*$H$5</f>
+        <v>1220400</v>
       </c>
       <c r="E48" cm="1">
         <f t="array" ref="E48">INDEX($L$7:$L$23,MOD(A48,17)+1,1)</f>
         <v>42</v>
       </c>
       <c r="O48">
+        <f>B48</f>
+        <v>14</v>
+      </c>
+      <c r="P48">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="R48">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="S48">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.4">
@@ -4463,32 +4529,32 @@
         <v>43</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49">
-        <f t="shared" si="0"/>
-        <v>615600</v>
+        <f>B49*$H$4+C49*$H$5</f>
+        <v>1134000</v>
       </c>
       <c r="E49" cm="1">
         <f t="array" ref="E49">INDEX($L$7:$L$23,MOD(A49,17)+1,1)</f>
         <v>39</v>
       </c>
       <c r="O49">
+        <f>B49</f>
+        <v>13</v>
+      </c>
+      <c r="P49">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="R49">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S49">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.4">
@@ -4496,32 +4562,32 @@
         <v>44</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50">
-        <f t="shared" si="0"/>
-        <v>529200</v>
+        <f>B50*$H$4+C50*$H$5</f>
+        <v>1047600</v>
       </c>
       <c r="E50" cm="1">
         <f t="array" ref="E50">INDEX($L$7:$L$23,MOD(A50,17)+1,1)</f>
         <v>20</v>
       </c>
       <c r="O50">
+        <f>B50</f>
+        <v>12</v>
+      </c>
+      <c r="P50">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="R50">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S50">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
@@ -4529,32 +4595,32 @@
         <v>45</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
       <c r="D51">
-        <f t="shared" si="0"/>
-        <v>442800</v>
+        <f>B51*$H$4+C51*$H$5</f>
+        <v>961200</v>
       </c>
       <c r="E51" cm="1">
         <f t="array" ref="E51">INDEX($L$7:$L$23,MOD(A51,17)+1,1)</f>
         <v>17</v>
       </c>
       <c r="O51">
+        <f>B51</f>
+        <v>11</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="R51">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S51">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.4">
@@ -4562,55 +4628,451 @@
         <v>46</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52">
-        <f t="shared" si="0"/>
-        <v>442800</v>
+        <f>B52*$H$4+C52*$H$5</f>
+        <v>874800</v>
       </c>
       <c r="E52" cm="1">
         <f t="array" ref="E52">INDEX($L$7:$L$23,MOD(A52,17)+1,1)</f>
         <v>35</v>
       </c>
       <c r="O52">
+        <f>B52</f>
+        <v>10</v>
+      </c>
+      <c r="P52">
         <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="R52">
+        <v>8</v>
+      </c>
+      <c r="S52">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>47</v>
+      </c>
+      <c r="B53">
+        <v>9</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <f>B53*$H$4+C53*$H$5</f>
+        <v>788400</v>
+      </c>
+      <c r="E53" cm="1">
+        <f t="array" ref="E53">INDEX($L$7:$L$23,MOD(A53,17)+1,1)</f>
+        <v>23</v>
+      </c>
+      <c r="O53">
+        <f>B53</f>
+        <v>9</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="R53">
+        <v>7</v>
+      </c>
+      <c r="S53">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>48</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <f>B54*$H$4+C54*$H$5</f>
+        <v>702000</v>
+      </c>
+      <c r="E54" cm="1">
+        <f t="array" ref="E54">INDEX($L$7:$L$23,MOD(A54,17)+1,1)</f>
+        <v>23</v>
+      </c>
+      <c r="O54">
+        <f>B54</f>
+        <v>8</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="R54">
+        <v>6</v>
+      </c>
+      <c r="S54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>49</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <f>B55*$H$4+C55*$H$5</f>
+        <v>615600</v>
+      </c>
+      <c r="E55" cm="1">
+        <f t="array" ref="E55">INDEX($L$7:$L$23,MOD(A55,17)+1,1)</f>
+        <v>25</v>
+      </c>
+      <c r="O55">
+        <f>B55</f>
+        <v>7</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R55">
         <v>5</v>
       </c>
-      <c r="P52">
+      <c r="S55">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>50</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <f>B56*$H$4+C56*$H$5</f>
+        <v>529200</v>
+      </c>
+      <c r="E56" cm="1">
+        <f t="array" ref="E56">INDEX($L$7:$L$23,MOD(A56,17)+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="O56">
+        <f>B56</f>
+        <v>6</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="R56">
+        <v>4</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>51</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <f>B57*$H$4+C57*$H$5</f>
+        <v>442800</v>
+      </c>
+      <c r="E57" cm="1">
+        <f t="array" ref="E57">INDEX($L$7:$L$23,MOD(A57,17)+1,1)</f>
+        <v>19</v>
+      </c>
+      <c r="O57">
+        <f>B57</f>
+        <v>5</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="R57">
+        <v>3</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>52</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <f>B58*$H$4+C58*$H$5</f>
+        <v>442800</v>
+      </c>
+      <c r="E58" cm="1">
+        <f t="array" ref="E58">INDEX($L$7:$L$23,MOD(A58,17)+1,1)</f>
+        <v>24</v>
+      </c>
+      <c r="O58">
+        <f>B58</f>
+        <v>5</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="R58">
+        <v>2</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>53</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <f>B59*$H$4+C59*$H$5</f>
+        <v>345600</v>
+      </c>
+      <c r="E59" cm="1">
+        <f t="array" ref="E59">INDEX($L$7:$L$23,MOD(A59,17)+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="O59">
+        <f t="shared" ref="O59:O68" si="2">B59</f>
+        <v>4</v>
+      </c>
+      <c r="P59">
+        <f t="shared" ref="P59:P68" si="3">E59</f>
+        <v>26</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>54</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <f>B60*$H$4+C60*$H$5</f>
+        <v>259200</v>
+      </c>
+      <c r="E60" cm="1">
+        <f t="array" ref="E60">INDEX($L$7:$L$23,MOD(A60,17)+1,1)</f>
+        <v>22</v>
+      </c>
+      <c r="O60">
         <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>55</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <f>B61*$H$4+C61*$H$5</f>
+        <v>259200</v>
+      </c>
+      <c r="E61" cm="1">
+        <f t="array" ref="E61">INDEX($L$7:$L$23,MOD(A61,17)+1,1)</f>
+        <v>30</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>56</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <f>B62*$H$4+C62*$H$5</f>
+        <v>172800</v>
+      </c>
+      <c r="E62" cm="1">
+        <f t="array" ref="E62">INDEX($L$7:$L$23,MOD(A62,17)+1,1)</f>
         <v>35</v>
       </c>
-      <c r="R52">
-        <v>3</v>
-      </c>
-      <c r="S52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="R53">
+      <c r="O62">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="S53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="R54">
-        <v>1</v>
-      </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="R55">
-        <v>0</v>
-      </c>
-      <c r="S55">
+      <c r="P62">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="O63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="O64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="15:19" x14ac:dyDescent="0.4">
+      <c r="O65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="15:19" x14ac:dyDescent="0.4">
+      <c r="O66">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="15:19" x14ac:dyDescent="0.4">
+      <c r="O67">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="15:19" x14ac:dyDescent="0.4">
+      <c r="O68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4622,611 +5084,681 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3E5EB3-BA15-47C5-9667-8B5EE7F07FA1}">
-  <dimension ref="A3:B62"/>
+  <dimension ref="A4:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:B48"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B60" sqref="A4:B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="str">
+        <f>Sheet1!$D6</f>
+        <v>Offset</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Sheet1!$E6</f>
+        <v>HRV</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5">
         <f>Sheet1!$D7</f>
-        <v>4150800</v>
-      </c>
-      <c r="B3">
+        <v>4586400</v>
+      </c>
+      <c r="B5">
         <f>Sheet1!$E7</f>
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6">
         <f>Sheet1!$D8</f>
-        <v>3985200</v>
-      </c>
-      <c r="B4">
+        <v>4500000</v>
+      </c>
+      <c r="B6">
         <f>Sheet1!$E8</f>
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7">
         <f>Sheet1!$D9</f>
-        <v>3988800</v>
-      </c>
-      <c r="B5">
+        <v>4413600</v>
+      </c>
+      <c r="B7">
         <f>Sheet1!$E9</f>
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8">
         <f>Sheet1!$D10</f>
-        <v>3996000</v>
-      </c>
-      <c r="B6">
+        <v>4327200</v>
+      </c>
+      <c r="B8">
         <f>Sheet1!$E10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9">
         <f>Sheet1!$D11</f>
-        <v>3895200</v>
-      </c>
-      <c r="B7">
+        <v>4240800</v>
+      </c>
+      <c r="B9">
         <f>Sheet1!$E11</f>
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10">
         <f>Sheet1!$D12</f>
-        <v>3812400</v>
-      </c>
-      <c r="B8">
+        <v>4154400</v>
+      </c>
+      <c r="B10">
         <f>Sheet1!$E12</f>
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11">
         <f>Sheet1!$D13</f>
-        <v>3726000</v>
-      </c>
-      <c r="B9">
+        <v>4064400</v>
+      </c>
+      <c r="B11">
         <f>Sheet1!$E13</f>
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12">
         <f>Sheet1!$D14</f>
-        <v>3639600</v>
-      </c>
-      <c r="B10">
+        <v>3985200</v>
+      </c>
+      <c r="B12">
         <f>Sheet1!$E14</f>
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13">
         <f>Sheet1!$D15</f>
-        <v>3553200</v>
-      </c>
-      <c r="B11">
+        <v>3988800</v>
+      </c>
+      <c r="B13">
         <f>Sheet1!$E15</f>
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14">
         <f>Sheet1!$D16</f>
-        <v>3466800</v>
-      </c>
-      <c r="B12">
+        <v>3996000</v>
+      </c>
+      <c r="B14">
         <f>Sheet1!$E16</f>
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15">
         <f>Sheet1!$D17</f>
-        <v>3380400</v>
-      </c>
-      <c r="B13">
+        <v>3895200</v>
+      </c>
+      <c r="B15">
         <f>Sheet1!$E17</f>
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16">
         <f>Sheet1!$D18</f>
-        <v>3294000</v>
-      </c>
-      <c r="B14">
+        <v>3812400</v>
+      </c>
+      <c r="B16">
         <f>Sheet1!$E18</f>
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17">
         <f>Sheet1!$D19</f>
-        <v>3207600</v>
-      </c>
-      <c r="B15">
+        <v>3726000</v>
+      </c>
+      <c r="B17">
         <f>Sheet1!$E19</f>
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18">
         <f>Sheet1!$D20</f>
-        <v>3121200</v>
-      </c>
-      <c r="B16">
+        <v>3639600</v>
+      </c>
+      <c r="B18">
         <f>Sheet1!$E20</f>
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19">
         <f>Sheet1!$D21</f>
-        <v>3034800</v>
-      </c>
-      <c r="B17">
+        <v>3553200</v>
+      </c>
+      <c r="B19">
         <f>Sheet1!$E21</f>
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20">
         <f>Sheet1!$D22</f>
-        <v>2948400</v>
-      </c>
-      <c r="B18">
+        <v>3466800</v>
+      </c>
+      <c r="B20">
         <f>Sheet1!$E22</f>
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21">
         <f>Sheet1!$D23</f>
-        <v>2862000</v>
-      </c>
-      <c r="B19">
+        <v>3380400</v>
+      </c>
+      <c r="B21">
         <f>Sheet1!$E23</f>
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22">
         <f>Sheet1!$D24</f>
-        <v>2775600</v>
-      </c>
-      <c r="B20">
+        <v>3294000</v>
+      </c>
+      <c r="B22">
         <f>Sheet1!$E24</f>
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23">
         <f>Sheet1!$D25</f>
-        <v>2689200</v>
-      </c>
-      <c r="B21">
+        <v>3207600</v>
+      </c>
+      <c r="B23">
         <f>Sheet1!$E25</f>
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24">
         <f>Sheet1!$D26</f>
-        <v>2602800</v>
-      </c>
-      <c r="B22">
+        <v>3121200</v>
+      </c>
+      <c r="B24">
         <f>Sheet1!$E26</f>
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25">
         <f>Sheet1!$D27</f>
-        <v>2516400</v>
-      </c>
-      <c r="B23">
+        <v>3034800</v>
+      </c>
+      <c r="B25">
         <f>Sheet1!$E27</f>
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26">
         <f>Sheet1!$D28</f>
-        <v>2430000</v>
-      </c>
-      <c r="B24">
+        <v>2948400</v>
+      </c>
+      <c r="B26">
         <f>Sheet1!$E28</f>
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27">
         <f>Sheet1!$D29</f>
-        <v>2343600</v>
-      </c>
-      <c r="B25">
+        <v>2862000</v>
+      </c>
+      <c r="B27">
         <f>Sheet1!$E29</f>
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28">
         <f>Sheet1!$D30</f>
-        <v>2257200</v>
-      </c>
-      <c r="B26">
+        <v>2775600</v>
+      </c>
+      <c r="B28">
         <f>Sheet1!$E30</f>
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29">
         <f>Sheet1!$D31</f>
-        <v>2170800</v>
-      </c>
-      <c r="B27">
+        <v>2689200</v>
+      </c>
+      <c r="B29">
         <f>Sheet1!$E31</f>
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30">
         <f>Sheet1!$D32</f>
-        <v>2170800</v>
-      </c>
-      <c r="B28">
+        <v>2602800</v>
+      </c>
+      <c r="B30">
         <f>Sheet1!$E32</f>
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31">
         <f>Sheet1!$D33</f>
-        <v>2170800</v>
-      </c>
-      <c r="B29">
+        <v>2516400</v>
+      </c>
+      <c r="B31">
         <f>Sheet1!$E33</f>
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32">
         <f>Sheet1!$D34</f>
-        <v>1911600</v>
-      </c>
-      <c r="B30">
+        <v>2430000</v>
+      </c>
+      <c r="B32">
         <f>Sheet1!$E34</f>
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33">
         <f>Sheet1!$D35</f>
-        <v>1825200</v>
-      </c>
-      <c r="B31">
+        <v>2343600</v>
+      </c>
+      <c r="B33">
         <f>Sheet1!$E35</f>
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34">
         <f>Sheet1!$D36</f>
-        <v>1738800</v>
-      </c>
-      <c r="B32">
+        <v>2257200</v>
+      </c>
+      <c r="B34">
         <f>Sheet1!$E36</f>
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35">
         <f>Sheet1!$D37</f>
-        <v>1652400</v>
-      </c>
-      <c r="B33">
+        <v>2170800</v>
+      </c>
+      <c r="B35">
         <f>Sheet1!$E37</f>
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36">
         <f>Sheet1!$D38</f>
-        <v>1566000</v>
-      </c>
-      <c r="B34">
+        <v>2170800</v>
+      </c>
+      <c r="B36">
         <f>Sheet1!$E38</f>
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37">
         <f>Sheet1!$D39</f>
-        <v>1479600</v>
-      </c>
-      <c r="B35">
+        <v>2170800</v>
+      </c>
+      <c r="B37">
         <f>Sheet1!$E39</f>
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A36">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38">
         <f>Sheet1!$D40</f>
-        <v>1393200</v>
-      </c>
-      <c r="B36">
+        <v>1911600</v>
+      </c>
+      <c r="B38">
         <f>Sheet1!$E40</f>
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A37">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39">
         <f>Sheet1!$D41</f>
-        <v>1306800</v>
-      </c>
-      <c r="B37">
+        <v>1825200</v>
+      </c>
+      <c r="B39">
         <f>Sheet1!$E41</f>
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40">
         <f>Sheet1!$D42</f>
-        <v>1220400</v>
-      </c>
-      <c r="B38">
+        <v>1738800</v>
+      </c>
+      <c r="B40">
         <f>Sheet1!$E42</f>
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41">
         <f>Sheet1!$D43</f>
-        <v>1134000</v>
-      </c>
-      <c r="B39">
+        <v>1652400</v>
+      </c>
+      <c r="B41">
         <f>Sheet1!$E43</f>
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42">
         <f>Sheet1!$D44</f>
-        <v>1047600</v>
-      </c>
-      <c r="B40">
+        <v>1566000</v>
+      </c>
+      <c r="B42">
         <f>Sheet1!$E44</f>
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43">
         <f>Sheet1!$D45</f>
-        <v>961200</v>
-      </c>
-      <c r="B41">
+        <v>1479600</v>
+      </c>
+      <c r="B43">
         <f>Sheet1!$E45</f>
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A42">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44">
         <f>Sheet1!$D46</f>
-        <v>874800</v>
-      </c>
-      <c r="B42">
+        <v>1393200</v>
+      </c>
+      <c r="B44">
         <f>Sheet1!$E46</f>
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A43">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45">
         <f>Sheet1!$D47</f>
-        <v>788400</v>
-      </c>
-      <c r="B43">
+        <v>1306800</v>
+      </c>
+      <c r="B45">
         <f>Sheet1!$E47</f>
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A44">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46">
         <f>Sheet1!$D48</f>
-        <v>702000</v>
-      </c>
-      <c r="B44">
+        <v>1220400</v>
+      </c>
+      <c r="B46">
         <f>Sheet1!$E48</f>
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47">
         <f>Sheet1!$D49</f>
-        <v>615600</v>
-      </c>
-      <c r="B45">
+        <v>1134000</v>
+      </c>
+      <c r="B47">
         <f>Sheet1!$E49</f>
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48">
         <f>Sheet1!$D50</f>
-        <v>529200</v>
-      </c>
-      <c r="B46">
+        <v>1047600</v>
+      </c>
+      <c r="B48">
         <f>Sheet1!$E50</f>
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A47">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49">
         <f>Sheet1!$D51</f>
-        <v>442800</v>
-      </c>
-      <c r="B47">
+        <v>961200</v>
+      </c>
+      <c r="B49">
         <f>Sheet1!$E51</f>
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A48">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50">
         <f>Sheet1!$D52</f>
-        <v>442800</v>
-      </c>
-      <c r="B48">
+        <v>874800</v>
+      </c>
+      <c r="B50">
         <f>Sheet1!$E52</f>
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A49">
-        <f>Sheet1!$D53</f>
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <f>Sheet1!$E53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A50">
-        <f>Sheet1!$D54</f>
-        <v>0</v>
-      </c>
-      <c r="B50">
-        <f>Sheet1!$E54</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51">
-        <f>Sheet1!$D55</f>
-        <v>0</v>
+        <f>Sheet1!$D53</f>
+        <v>788400</v>
       </c>
       <c r="B51">
-        <f>Sheet1!$E55</f>
-        <v>0</v>
+        <f>Sheet1!$E53</f>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52">
-        <f>Sheet1!$D56</f>
-        <v>0</v>
+        <f>Sheet1!$D54</f>
+        <v>702000</v>
       </c>
       <c r="B52">
-        <f>Sheet1!$E56</f>
-        <v>0</v>
+        <f>Sheet1!$E54</f>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53">
-        <f>Sheet1!$D57</f>
-        <v>0</v>
+        <f>Sheet1!$D55</f>
+        <v>615600</v>
       </c>
       <c r="B53">
-        <f>Sheet1!$E57</f>
-        <v>0</v>
+        <f>Sheet1!$E55</f>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54">
-        <f>Sheet1!$D58</f>
-        <v>0</v>
+        <f>Sheet1!$D56</f>
+        <v>529200</v>
       </c>
       <c r="B54">
-        <f>Sheet1!$E58</f>
-        <v>0</v>
+        <f>Sheet1!$E56</f>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55">
-        <f>Sheet1!$D59</f>
-        <v>0</v>
+        <f>Sheet1!$D57</f>
+        <v>442800</v>
       </c>
       <c r="B55">
-        <f>Sheet1!$E59</f>
-        <v>0</v>
+        <f>Sheet1!$E57</f>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56">
-        <f>Sheet1!$D60</f>
-        <v>0</v>
+        <f>Sheet1!$D58</f>
+        <v>442800</v>
       </c>
       <c r="B56">
-        <f>Sheet1!$E60</f>
-        <v>0</v>
+        <f>Sheet1!$E58</f>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57">
-        <f>Sheet1!$D61</f>
-        <v>0</v>
+        <f>Sheet1!$D59</f>
+        <v>345600</v>
       </c>
       <c r="B57">
-        <f>Sheet1!$E61</f>
-        <v>0</v>
+        <f>Sheet1!$E59</f>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A58">
-        <f>Sheet1!$D62</f>
-        <v>0</v>
+        <f>Sheet1!$D60</f>
+        <v>259200</v>
       </c>
       <c r="B58">
-        <f>Sheet1!$E62</f>
-        <v>0</v>
+        <f>Sheet1!$E60</f>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A59">
-        <f>Sheet1!$D63</f>
-        <v>0</v>
+        <f>Sheet1!$D61</f>
+        <v>259200</v>
       </c>
       <c r="B59">
-        <f>Sheet1!$E63</f>
-        <v>0</v>
+        <f>Sheet1!$E61</f>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60">
-        <f>Sheet1!$D64</f>
-        <v>0</v>
+        <f>Sheet1!$D62</f>
+        <v>172800</v>
       </c>
       <c r="B60">
-        <f>Sheet1!$E64</f>
-        <v>0</v>
+        <f>Sheet1!$E62</f>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61">
-        <f>Sheet1!$D65</f>
+        <f>Sheet1!$D63</f>
         <v>0</v>
       </c>
       <c r="B61">
-        <f>Sheet1!$E65</f>
+        <f>Sheet1!$E63</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A62">
+        <f>Sheet1!$D64</f>
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <f>Sheet1!$E64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <f>Sheet1!$D65</f>
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <f>Sheet1!$E65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64">
         <f>Sheet1!$D66</f>
         <v>0</v>
       </c>
-      <c r="B62">
+      <c r="B64">
         <f>Sheet1!$E66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <f>Sheet1!$D67</f>
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <f>Sheet1!$E67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <f>Sheet1!$D68</f>
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <f>Sheet1!$E68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <f>Sheet1!$D69</f>
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <f>Sheet1!$E69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <f>Sheet1!$D70</f>
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <f>Sheet1!$E70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <f>Sheet1!$D71</f>
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <f>Sheet1!$E71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <f>Sheet1!$D72</f>
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <f>Sheet1!$E72</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to gance gen and history. Need to look at number of points in each range of regression
</commit_message>
<xml_diff>
--- a/HRV trend test data.xlsx
+++ b/HRV trend test data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcte\Non OneDrive Docs\GitHub\HRVApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmcternan/Documents/Git code/HRVApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A81150-0DA2-4D51-B178-37F2CA86C33C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF7ACD-104F-804F-9408-7C5D6DE6A8E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5057" yWindow="1911" windowWidth="27009" windowHeight="16603" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="500" windowWidth="27000" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Assume base date comes from app as today in UTC time. Data here is always an offset</t>
   </si>
@@ -100,18 +100,33 @@
   <si>
     <t>AVG</t>
   </si>
+  <si>
+    <t>26.000000, 26.000000, 35.000000, 0.000000, 0.000000</t>
+  </si>
+  <si>
+    <t>35.000000, 23.000000, 23.000000, 25.000000, 26.000000, 21.500000, 26.000000, 26.000000, 35.000000, 0.000000, 0.000000]</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,11 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,7 +175,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -842,7 +858,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1222,10 +1238,10 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>0</c:v>
@@ -3005,33 +3021,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="AG62" sqref="AG62"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3043,7 +3059,7 @@
         <v>86400</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G5" t="s">
         <v>9</v>
       </c>
@@ -3052,7 +3068,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3084,7 +3100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3106,11 +3122,11 @@
         <v>19</v>
       </c>
       <c r="O7">
-        <f>B7</f>
+        <f t="shared" ref="O7:O38" si="1">B7</f>
         <v>53</v>
       </c>
       <c r="P7">
-        <f>E7</f>
+        <f t="shared" ref="P7:P13" si="2">E7</f>
         <v>24</v>
       </c>
       <c r="R7" s="1">
@@ -3120,7 +3136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3142,11 +3158,11 @@
         <v>24</v>
       </c>
       <c r="O8">
-        <f>B8</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="P8">
-        <f>E8</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="R8" s="1">
@@ -3156,7 +3172,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3178,11 +3194,11 @@
         <v>26</v>
       </c>
       <c r="O9">
-        <f>B9</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="P9">
-        <f>E9</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="R9" s="1">
@@ -3192,7 +3208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3214,11 +3230,11 @@
         <v>22</v>
       </c>
       <c r="O10">
-        <f>B10</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="P10">
-        <f>E10</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="R10" s="1">
@@ -3228,7 +3244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3250,11 +3266,11 @@
         <v>30</v>
       </c>
       <c r="O11">
-        <f>B11</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="P11">
-        <f>E11</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R11" s="1">
@@ -3264,7 +3280,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -3286,11 +3302,11 @@
         <v>35</v>
       </c>
       <c r="O12">
-        <f>B12</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="P12">
-        <f>E12</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="R12" s="1">
@@ -3300,7 +3316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -3311,7 +3327,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <f>B13*$H$4+C13*$H$5</f>
+        <f t="shared" ref="D13:D44" si="3">B13*$H$4+C13*$H$5</f>
         <v>4064400</v>
       </c>
       <c r="E13" cm="1">
@@ -3322,11 +3338,11 @@
         <v>38</v>
       </c>
       <c r="O13">
-        <f>B13</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="P13">
-        <f>E13</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="R13">
@@ -3336,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -3347,7 +3363,7 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <f>B14*$H$4+C14*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3985200</v>
       </c>
       <c r="E14" cm="1">
@@ -3358,11 +3374,11 @@
         <v>43</v>
       </c>
       <c r="O14">
-        <f>B14</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:P58" si="1">E14</f>
+        <f t="shared" ref="P14:P58" si="4">E14</f>
         <v>42</v>
       </c>
       <c r="R14">
@@ -3372,7 +3388,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -3383,7 +3399,7 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <f>B15*$H$4+C15*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3988800</v>
       </c>
       <c r="E15" cm="1">
@@ -3394,11 +3410,11 @@
         <v>42</v>
       </c>
       <c r="O15">
-        <f>B15</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="P15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="R15">
@@ -3408,7 +3424,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -3419,7 +3435,7 @@
         <v>6</v>
       </c>
       <c r="D16">
-        <f>B16*$H$4+C16*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3996000</v>
       </c>
       <c r="E16" cm="1">
@@ -3430,11 +3446,11 @@
         <v>39</v>
       </c>
       <c r="O16">
-        <f>B16</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="P16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="R16">
@@ -3444,7 +3460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -3455,7 +3471,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <f>B17*$H$4+C17*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3895200</v>
       </c>
       <c r="E17" cm="1">
@@ -3466,11 +3482,11 @@
         <v>20</v>
       </c>
       <c r="O17">
-        <f>B17</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="P17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="R17">
@@ -3480,7 +3496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -3491,7 +3507,7 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <f>B18*$H$4+C18*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3812400</v>
       </c>
       <c r="E18" cm="1">
@@ -3502,11 +3518,11 @@
         <v>17</v>
       </c>
       <c r="O18">
-        <f>B18</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="P18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="R18">
@@ -3516,7 +3532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -3527,7 +3543,7 @@
         <v>3</v>
       </c>
       <c r="D19">
-        <f>B19*$H$4+C19*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3726000</v>
       </c>
       <c r="E19" cm="1">
@@ -3538,11 +3554,11 @@
         <v>35</v>
       </c>
       <c r="O19">
-        <f>B19</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="P19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R19">
@@ -3552,7 +3568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -3563,7 +3579,7 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <f>B20*$H$4+C20*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3639600</v>
       </c>
       <c r="E20" cm="1">
@@ -3574,11 +3590,11 @@
         <v>23</v>
       </c>
       <c r="O20">
-        <f>B20</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="P20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R20">
@@ -3588,7 +3604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -3599,7 +3615,7 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <f>B21*$H$4+C21*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3553200</v>
       </c>
       <c r="E21" cm="1">
@@ -3610,11 +3626,11 @@
         <v>23</v>
       </c>
       <c r="O21">
-        <f>B21</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="P21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="R21">
@@ -3624,7 +3640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -3635,7 +3651,7 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <f>B22*$H$4+C22*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3466800</v>
       </c>
       <c r="E22" cm="1">
@@ -3646,11 +3662,11 @@
         <v>25</v>
       </c>
       <c r="O22">
-        <f>B22</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="P22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="R22">
@@ -3660,7 +3676,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -3671,7 +3687,7 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <f>B23*$H$4+C23*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3380400</v>
       </c>
       <c r="E23" cm="1">
@@ -3682,11 +3698,11 @@
         <v>26</v>
       </c>
       <c r="O23">
-        <f>B23</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="P23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="R23">
@@ -3696,7 +3712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -3707,7 +3723,7 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f>B24*$H$4+C24*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3294000</v>
       </c>
       <c r="E24" cm="1">
@@ -3718,11 +3734,11 @@
         <v>27</v>
       </c>
       <c r="O24">
-        <f>B24</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="P24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="R24">
@@ -3732,7 +3748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -3743,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <f>B25*$H$4+C25*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3207600</v>
       </c>
       <c r="E25" cm="1">
@@ -3751,11 +3767,11 @@
         <v>26</v>
       </c>
       <c r="O25">
-        <f>B25</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="P25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="R25">
@@ -3765,7 +3781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -3776,7 +3792,7 @@
         <v>3</v>
       </c>
       <c r="D26">
-        <f>B26*$H$4+C26*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3121200</v>
       </c>
       <c r="E26" cm="1">
@@ -3784,11 +3800,11 @@
         <v>22</v>
       </c>
       <c r="O26">
-        <f>B26</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="P26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="R26">
@@ -3798,7 +3814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -3809,7 +3825,7 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <f>B27*$H$4+C27*$H$5</f>
+        <f t="shared" si="3"/>
         <v>3034800</v>
       </c>
       <c r="E27" cm="1">
@@ -3817,11 +3833,11 @@
         <v>30</v>
       </c>
       <c r="O27">
-        <f>B27</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="P27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="R27">
@@ -3831,7 +3847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -3842,7 +3858,7 @@
         <v>3</v>
       </c>
       <c r="D28">
-        <f>B28*$H$4+C28*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2948400</v>
       </c>
       <c r="E28" cm="1">
@@ -3850,11 +3866,11 @@
         <v>35</v>
       </c>
       <c r="O28">
-        <f>B28</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="P28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="R28">
@@ -3864,7 +3880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
@@ -3875,7 +3891,7 @@
         <v>3</v>
       </c>
       <c r="D29">
-        <f>B29*$H$4+C29*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2862000</v>
       </c>
       <c r="E29" cm="1">
@@ -3883,11 +3899,11 @@
         <v>38</v>
       </c>
       <c r="O29">
-        <f>B29</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="R29">
@@ -3897,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
@@ -3908,7 +3924,7 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <f>B30*$H$4+C30*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2775600</v>
       </c>
       <c r="E30" cm="1">
@@ -3916,11 +3932,11 @@
         <v>43</v>
       </c>
       <c r="O30">
-        <f>B30</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="P30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="R30">
@@ -3930,7 +3946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
@@ -3941,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <f>B31*$H$4+C31*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2689200</v>
       </c>
       <c r="E31" cm="1">
@@ -3949,11 +3965,11 @@
         <v>42</v>
       </c>
       <c r="O31">
-        <f>B31</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="P31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="R31">
@@ -3963,7 +3979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
@@ -3974,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="D32">
-        <f>B32*$H$4+C32*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2602800</v>
       </c>
       <c r="E32" cm="1">
@@ -3982,11 +3998,11 @@
         <v>39</v>
       </c>
       <c r="O32">
-        <f>B32</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="R32">
@@ -3996,7 +4012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
@@ -4007,7 +4023,7 @@
         <v>3</v>
       </c>
       <c r="D33">
-        <f>B33*$H$4+C33*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2516400</v>
       </c>
       <c r="E33" cm="1">
@@ -4015,11 +4031,11 @@
         <v>20</v>
       </c>
       <c r="O33">
-        <f>B33</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="P33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="R33">
@@ -4029,7 +4045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
@@ -4040,7 +4056,7 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f>B34*$H$4+C34*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2430000</v>
       </c>
       <c r="E34" cm="1">
@@ -4048,11 +4064,11 @@
         <v>17</v>
       </c>
       <c r="O34">
-        <f>B34</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="P34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="R34">
@@ -4062,7 +4078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
@@ -4073,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="D35">
-        <f>B35*$H$4+C35*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2343600</v>
       </c>
       <c r="E35" cm="1">
@@ -4081,11 +4097,11 @@
         <v>35</v>
       </c>
       <c r="O35">
-        <f>B35</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="P35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="R35">
@@ -4095,7 +4111,7 @@
         <v>33.666668000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -4106,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="D36">
-        <f>B36*$H$4+C36*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2257200</v>
       </c>
       <c r="E36" cm="1">
@@ -4114,11 +4130,11 @@
         <v>23</v>
       </c>
       <c r="O36">
-        <f>B36</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="P36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R36">
@@ -4128,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>31</v>
       </c>
@@ -4139,7 +4155,7 @@
         <v>3</v>
       </c>
       <c r="D37">
-        <f>B37*$H$4+C37*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2170800</v>
       </c>
       <c r="E37" cm="1">
@@ -4147,11 +4163,11 @@
         <v>23</v>
       </c>
       <c r="O37">
-        <f>B37</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="P37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R37">
@@ -4161,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>32</v>
       </c>
@@ -4172,7 +4188,7 @@
         <v>3</v>
       </c>
       <c r="D38">
-        <f>B38*$H$4+C38*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2170800</v>
       </c>
       <c r="E38" cm="1">
@@ -4180,13 +4196,13 @@
         <v>25</v>
       </c>
       <c r="O38">
-        <f>B38</f>
-        <v>25</v>
-      </c>
-      <c r="P38">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="R38">
         <v>22</v>
       </c>
@@ -4194,7 +4210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>33</v>
       </c>
@@ -4205,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="D39">
-        <f>B39*$H$4+C39*$H$5</f>
+        <f t="shared" si="3"/>
         <v>2170800</v>
       </c>
       <c r="E39" cm="1">
@@ -4213,11 +4229,11 @@
         <v>26</v>
       </c>
       <c r="O39">
-        <f>B39</f>
+        <f t="shared" ref="O39:O58" si="5">B39</f>
         <v>25</v>
       </c>
       <c r="P39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="R39">
@@ -4227,7 +4243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>34</v>
       </c>
@@ -4238,7 +4254,7 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <f>B40*$H$4+C40*$H$5</f>
+        <f t="shared" si="3"/>
         <v>1911600</v>
       </c>
       <c r="E40" cm="1">
@@ -4246,11 +4262,11 @@
         <v>19</v>
       </c>
       <c r="O40">
-        <f>B40</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="P40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="R40">
@@ -4260,7 +4276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>35</v>
       </c>
@@ -4271,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="D41">
-        <f>B41*$H$4+C41*$H$5</f>
+        <f t="shared" si="3"/>
         <v>1825200</v>
       </c>
       <c r="E41" cm="1">
@@ -4279,11 +4295,11 @@
         <v>24</v>
       </c>
       <c r="O41">
-        <f>B41</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="P41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="R41">
@@ -4293,7 +4309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>36</v>
       </c>
@@ -4304,7 +4320,7 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <f>B42*$H$4+C42*$H$5</f>
+        <f t="shared" si="3"/>
         <v>1738800</v>
       </c>
       <c r="E42" cm="1">
@@ -4312,11 +4328,11 @@
         <v>26</v>
       </c>
       <c r="O42">
-        <f>B42</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="P42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="R42">
@@ -4326,7 +4342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>37</v>
       </c>
@@ -4337,7 +4353,7 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <f>B43*$H$4+C43*$H$5</f>
+        <f t="shared" si="3"/>
         <v>1652400</v>
       </c>
       <c r="E43" cm="1">
@@ -4345,11 +4361,11 @@
         <v>22</v>
       </c>
       <c r="O43">
-        <f>B43</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="P43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="R43">
@@ -4359,7 +4375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>38</v>
       </c>
@@ -4370,7 +4386,7 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <f>B44*$H$4+C44*$H$5</f>
+        <f t="shared" si="3"/>
         <v>1566000</v>
       </c>
       <c r="E44" cm="1">
@@ -4378,11 +4394,11 @@
         <v>30</v>
       </c>
       <c r="O44">
-        <f>B44</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="P44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="R44">
@@ -4392,7 +4408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>39</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>3</v>
       </c>
       <c r="D45">
-        <f>B45*$H$4+C45*$H$5</f>
+        <f t="shared" ref="D45:D62" si="6">B45*$H$4+C45*$H$5</f>
         <v>1479600</v>
       </c>
       <c r="E45" cm="1">
@@ -4411,11 +4427,11 @@
         <v>35</v>
       </c>
       <c r="O45">
-        <f>B45</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="P45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="R45">
@@ -4425,7 +4441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>40</v>
       </c>
@@ -4436,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="D46">
-        <f>B46*$H$4+C46*$H$5</f>
+        <f t="shared" si="6"/>
         <v>1393200</v>
       </c>
       <c r="E46" cm="1">
@@ -4444,11 +4460,11 @@
         <v>38</v>
       </c>
       <c r="O46">
-        <f>B46</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="P46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="R46">
@@ -4458,7 +4474,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>41</v>
       </c>
@@ -4469,7 +4485,7 @@
         <v>3</v>
       </c>
       <c r="D47">
-        <f>B47*$H$4+C47*$H$5</f>
+        <f t="shared" si="6"/>
         <v>1306800</v>
       </c>
       <c r="E47" cm="1">
@@ -4477,11 +4493,11 @@
         <v>43</v>
       </c>
       <c r="O47">
-        <f>B47</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="P47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="R47">
@@ -4491,7 +4507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>42</v>
       </c>
@@ -4502,7 +4518,7 @@
         <v>3</v>
       </c>
       <c r="D48">
-        <f>B48*$H$4+C48*$H$5</f>
+        <f t="shared" si="6"/>
         <v>1220400</v>
       </c>
       <c r="E48" cm="1">
@@ -4510,11 +4526,11 @@
         <v>42</v>
       </c>
       <c r="O48">
-        <f>B48</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="P48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="R48">
@@ -4524,7 +4540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>43</v>
       </c>
@@ -4535,7 +4551,7 @@
         <v>3</v>
       </c>
       <c r="D49">
-        <f>B49*$H$4+C49*$H$5</f>
+        <f t="shared" si="6"/>
         <v>1134000</v>
       </c>
       <c r="E49" cm="1">
@@ -4543,11 +4559,11 @@
         <v>39</v>
       </c>
       <c r="O49">
-        <f>B49</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="P49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="R49">
@@ -4557,7 +4573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>44</v>
       </c>
@@ -4568,7 +4584,7 @@
         <v>3</v>
       </c>
       <c r="D50">
-        <f>B50*$H$4+C50*$H$5</f>
+        <f t="shared" si="6"/>
         <v>1047600</v>
       </c>
       <c r="E50" cm="1">
@@ -4576,11 +4592,11 @@
         <v>20</v>
       </c>
       <c r="O50">
-        <f>B50</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="P50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="R50">
@@ -4590,7 +4606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>45</v>
       </c>
@@ -4601,7 +4617,7 @@
         <v>3</v>
       </c>
       <c r="D51">
-        <f>B51*$H$4+C51*$H$5</f>
+        <f t="shared" si="6"/>
         <v>961200</v>
       </c>
       <c r="E51" cm="1">
@@ -4609,11 +4625,11 @@
         <v>17</v>
       </c>
       <c r="O51">
-        <f>B51</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="P51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="R51">
@@ -4623,7 +4639,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>46</v>
       </c>
@@ -4634,7 +4650,7 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <f>B52*$H$4+C52*$H$5</f>
+        <f t="shared" si="6"/>
         <v>874800</v>
       </c>
       <c r="E52" cm="1">
@@ -4642,11 +4658,11 @@
         <v>35</v>
       </c>
       <c r="O52">
-        <f>B52</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="P52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="R52">
@@ -4656,7 +4672,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>47</v>
       </c>
@@ -4667,7 +4683,7 @@
         <v>3</v>
       </c>
       <c r="D53">
-        <f>B53*$H$4+C53*$H$5</f>
+        <f t="shared" si="6"/>
         <v>788400</v>
       </c>
       <c r="E53" cm="1">
@@ -4675,11 +4691,11 @@
         <v>23</v>
       </c>
       <c r="O53">
-        <f>B53</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="P53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R53">
@@ -4689,7 +4705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>48</v>
       </c>
@@ -4700,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="D54">
-        <f>B54*$H$4+C54*$H$5</f>
+        <f t="shared" si="6"/>
         <v>702000</v>
       </c>
       <c r="E54" cm="1">
@@ -4708,11 +4724,11 @@
         <v>23</v>
       </c>
       <c r="O54">
-        <f>B54</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="P54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="R54">
@@ -4722,7 +4738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>49</v>
       </c>
@@ -4733,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <f>B55*$H$4+C55*$H$5</f>
+        <f t="shared" si="6"/>
         <v>615600</v>
       </c>
       <c r="E55" cm="1">
@@ -4741,11 +4757,11 @@
         <v>25</v>
       </c>
       <c r="O55">
-        <f>B55</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="R55">
@@ -4755,7 +4771,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>50</v>
       </c>
@@ -4766,29 +4782,32 @@
         <v>3</v>
       </c>
       <c r="D56">
-        <f>B56*$H$4+C56*$H$5</f>
+        <f t="shared" si="6"/>
         <v>529200</v>
       </c>
       <c r="E56" cm="1">
         <f t="array" ref="E56">INDEX($L$7:$L$23,MOD(A56,17)+1,1)</f>
         <v>26</v>
       </c>
+      <c r="G56" t="s">
+        <v>16</v>
+      </c>
       <c r="O56">
-        <f>B56</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="R56">
         <v>4</v>
       </c>
       <c r="S56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>51</v>
       </c>
@@ -4799,29 +4818,32 @@
         <v>3</v>
       </c>
       <c r="D57">
-        <f>B57*$H$4+C57*$H$5</f>
+        <f t="shared" si="6"/>
         <v>442800</v>
       </c>
       <c r="E57" cm="1">
         <f t="array" ref="E57">INDEX($L$7:$L$23,MOD(A57,17)+1,1)</f>
         <v>19</v>
       </c>
+      <c r="F57">
+        <v>25</v>
+      </c>
       <c r="O57">
-        <f>B57</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="R57">
         <v>3</v>
       </c>
       <c r="S57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>52</v>
       </c>
@@ -4832,19 +4854,25 @@
         <v>3</v>
       </c>
       <c r="D58">
-        <f>B58*$H$4+C58*$H$5</f>
+        <f t="shared" si="6"/>
         <v>442800</v>
       </c>
       <c r="E58" cm="1">
         <f t="array" ref="E58">INDEX($L$7:$L$23,MOD(A58,17)+1,1)</f>
         <v>24</v>
       </c>
+      <c r="F58">
+        <v>26</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
       <c r="O58">
-        <f>B58</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="R58">
@@ -4854,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>53</v>
       </c>
@@ -4865,19 +4893,26 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <f>B59*$H$4+C59*$H$5</f>
+        <f t="shared" si="6"/>
         <v>345600</v>
       </c>
       <c r="E59" cm="1">
         <f t="array" ref="E59">INDEX($L$7:$L$23,MOD(A59,17)+1,1)</f>
         <v>26</v>
       </c>
+      <c r="F59">
+        <f>AVERAGE(E57,E58)</f>
+        <v>21.5</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
       <c r="O59">
-        <f t="shared" ref="O59:O68" si="2">B59</f>
+        <f t="shared" ref="O59:O68" si="7">B59</f>
         <v>4</v>
       </c>
       <c r="P59">
-        <f t="shared" ref="P59:P68" si="3">E59</f>
+        <f t="shared" ref="P59:P68" si="8">E59</f>
         <v>26</v>
       </c>
       <c r="R59">
@@ -4887,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>54</v>
       </c>
@@ -4898,19 +4933,26 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <f>B60*$H$4+C60*$H$5</f>
+        <f t="shared" si="6"/>
         <v>259200</v>
       </c>
       <c r="E60" cm="1">
         <f t="array" ref="E60">INDEX($L$7:$L$23,MOD(A60,17)+1,1)</f>
         <v>22</v>
       </c>
+      <c r="F60">
+        <f>E59</f>
+        <v>26</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
       <c r="O60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="P60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="R60">
@@ -4920,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>55</v>
       </c>
@@ -4931,19 +4973,29 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <f>B61*$H$4+C61*$H$5</f>
+        <f t="shared" si="6"/>
         <v>259200</v>
       </c>
       <c r="E61" cm="1">
         <f t="array" ref="E61">INDEX($L$7:$L$23,MOD(A61,17)+1,1)</f>
         <v>30</v>
       </c>
+      <c r="F61">
+        <f>AVERAGE(E60,E61)</f>
+        <v>26</v>
+      </c>
+      <c r="G61">
+        <v>4</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="O61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="P61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="R61">
@@ -4953,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>56</v>
       </c>
@@ -4964,19 +5016,25 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <f>B62*$H$4+C62*$H$5</f>
+        <f t="shared" si="6"/>
         <v>172800</v>
       </c>
       <c r="E62" cm="1">
         <f t="array" ref="E62">INDEX($L$7:$L$23,MOD(A62,17)+1,1)</f>
         <v>35</v>
       </c>
+      <c r="F62">
+        <v>35</v>
+      </c>
+      <c r="G62">
+        <v>5</v>
+      </c>
       <c r="O62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="P62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="R62">
@@ -4986,13 +5044,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>6</v>
+      </c>
       <c r="O63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R63">
@@ -5002,13 +5066,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>7</v>
+      </c>
       <c r="O64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R64">
@@ -5018,13 +5088,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="15:19" x14ac:dyDescent="0.4">
+    <row r="65" spans="6:20" x14ac:dyDescent="0.2">
       <c r="O65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R65">
@@ -5034,13 +5104,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="15:19" x14ac:dyDescent="0.4">
+    <row r="66" spans="6:20" x14ac:dyDescent="0.2">
+      <c r="F66" cm="1">
+        <f t="array" ref="F66:G66">LINEST(F58:F62,G58:G62,TRUE)</f>
+        <v>2.2500000000000004</v>
+      </c>
+      <c r="G66">
+        <v>20.149999999999999</v>
+      </c>
       <c r="O66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R66">
@@ -5050,13 +5127,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="15:19" x14ac:dyDescent="0.4">
+    <row r="67" spans="6:20" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <f>G66+7*F66</f>
+        <v>35.900000000000006</v>
+      </c>
       <c r="O67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R67">
@@ -5066,14 +5147,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="15:19" x14ac:dyDescent="0.4">
+    <row r="68" spans="6:20" x14ac:dyDescent="0.2">
       <c r="O68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P68">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="F69" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="6:20" x14ac:dyDescent="0.2">
+      <c r="S72" cm="1">
+        <f t="array" ref="S72:T72">LINEST(S53:S59,R53:R59,TRUE)</f>
+        <v>5.2857142857142847</v>
+      </c>
+      <c r="T72">
+        <v>-0.28571428571428115</v>
+      </c>
+    </row>
+    <row r="73" spans="6:20" x14ac:dyDescent="0.2">
+      <c r="S73" cm="1">
+        <f t="array" ref="S73:T73">LINEST(S52:S58,R53:R59,TRUE)</f>
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="T73">
+        <v>8.571428571428573</v>
       </c>
     </row>
   </sheetData>
@@ -5086,13 +5190,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3E5EB3-BA15-47C5-9667-8B5EE7F07FA1}">
   <dimension ref="A4:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B60" sqref="A4:B60"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Sheet1!$D6</f>
         <v>Offset</v>
@@ -5102,7 +5206,7 @@
         <v>HRV</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>Sheet1!$D7</f>
         <v>4586400</v>
@@ -5112,7 +5216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>Sheet1!$D8</f>
         <v>4500000</v>
@@ -5122,7 +5226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>Sheet1!$D9</f>
         <v>4413600</v>
@@ -5132,7 +5236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>Sheet1!$D10</f>
         <v>4327200</v>
@@ -5142,7 +5246,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>Sheet1!$D11</f>
         <v>4240800</v>
@@ -5152,7 +5256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>Sheet1!$D12</f>
         <v>4154400</v>
@@ -5162,7 +5266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f>Sheet1!$D13</f>
         <v>4064400</v>
@@ -5172,7 +5276,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>Sheet1!$D14</f>
         <v>3985200</v>
@@ -5182,7 +5286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>Sheet1!$D15</f>
         <v>3988800</v>
@@ -5192,7 +5296,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <f>Sheet1!$D16</f>
         <v>3996000</v>
@@ -5202,7 +5306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>Sheet1!$D17</f>
         <v>3895200</v>
@@ -5212,7 +5316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <f>Sheet1!$D18</f>
         <v>3812400</v>
@@ -5222,7 +5326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>Sheet1!$D19</f>
         <v>3726000</v>
@@ -5232,7 +5336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>Sheet1!$D20</f>
         <v>3639600</v>
@@ -5242,7 +5346,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>Sheet1!$D21</f>
         <v>3553200</v>
@@ -5252,7 +5356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>Sheet1!$D22</f>
         <v>3466800</v>
@@ -5262,7 +5366,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>Sheet1!$D23</f>
         <v>3380400</v>
@@ -5272,7 +5376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>Sheet1!$D24</f>
         <v>3294000</v>
@@ -5282,7 +5386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>Sheet1!$D25</f>
         <v>3207600</v>
@@ -5292,7 +5396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>Sheet1!$D26</f>
         <v>3121200</v>
@@ -5302,7 +5406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>Sheet1!$D27</f>
         <v>3034800</v>
@@ -5312,7 +5416,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>Sheet1!$D28</f>
         <v>2948400</v>
@@ -5322,7 +5426,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>Sheet1!$D29</f>
         <v>2862000</v>
@@ -5332,7 +5436,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>Sheet1!$D30</f>
         <v>2775600</v>
@@ -5342,7 +5446,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>Sheet1!$D31</f>
         <v>2689200</v>
@@ -5352,7 +5456,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>Sheet1!$D32</f>
         <v>2602800</v>
@@ -5362,7 +5466,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>Sheet1!$D33</f>
         <v>2516400</v>
@@ -5372,7 +5476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>Sheet1!$D34</f>
         <v>2430000</v>
@@ -5382,7 +5486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>Sheet1!$D35</f>
         <v>2343600</v>
@@ -5392,7 +5496,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>Sheet1!$D36</f>
         <v>2257200</v>
@@ -5402,7 +5506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>Sheet1!$D37</f>
         <v>2170800</v>
@@ -5412,7 +5516,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>Sheet1!$D38</f>
         <v>2170800</v>
@@ -5422,7 +5526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>Sheet1!$D39</f>
         <v>2170800</v>
@@ -5432,7 +5536,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>Sheet1!$D40</f>
         <v>1911600</v>
@@ -5442,7 +5546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>Sheet1!$D41</f>
         <v>1825200</v>
@@ -5452,7 +5556,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>Sheet1!$D42</f>
         <v>1738800</v>
@@ -5462,7 +5566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <f>Sheet1!$D43</f>
         <v>1652400</v>
@@ -5472,7 +5576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <f>Sheet1!$D44</f>
         <v>1566000</v>
@@ -5482,7 +5586,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <f>Sheet1!$D45</f>
         <v>1479600</v>
@@ -5492,7 +5596,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <f>Sheet1!$D46</f>
         <v>1393200</v>
@@ -5502,7 +5606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>Sheet1!$D47</f>
         <v>1306800</v>
@@ -5512,7 +5616,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <f>Sheet1!$D48</f>
         <v>1220400</v>
@@ -5522,7 +5626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <f>Sheet1!$D49</f>
         <v>1134000</v>
@@ -5532,7 +5636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <f>Sheet1!$D50</f>
         <v>1047600</v>
@@ -5542,7 +5646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <f>Sheet1!$D51</f>
         <v>961200</v>
@@ -5552,7 +5656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <f>Sheet1!$D52</f>
         <v>874800</v>
@@ -5562,7 +5666,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <f>Sheet1!$D53</f>
         <v>788400</v>
@@ -5572,7 +5676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <f>Sheet1!$D54</f>
         <v>702000</v>
@@ -5582,7 +5686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <f>Sheet1!$D55</f>
         <v>615600</v>
@@ -5592,7 +5696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <f>Sheet1!$D56</f>
         <v>529200</v>
@@ -5602,7 +5706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <f>Sheet1!$D57</f>
         <v>442800</v>
@@ -5612,7 +5716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <f>Sheet1!$D58</f>
         <v>442800</v>
@@ -5622,7 +5726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <f>Sheet1!$D59</f>
         <v>345600</v>
@@ -5632,7 +5736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <f>Sheet1!$D60</f>
         <v>259200</v>
@@ -5642,7 +5746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <f>Sheet1!$D61</f>
         <v>259200</v>
@@ -5652,7 +5756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <f>Sheet1!$D62</f>
         <v>172800</v>
@@ -5662,7 +5766,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <f>Sheet1!$D63</f>
         <v>0</v>
@@ -5672,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>Sheet1!$D64</f>
         <v>0</v>
@@ -5682,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <f>Sheet1!$D65</f>
         <v>0</v>
@@ -5692,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <f>Sheet1!$D66</f>
         <v>0</v>
@@ -5702,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <f>Sheet1!$D67</f>
         <v>0</v>
@@ -5712,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <f>Sheet1!$D68</f>
         <v>0</v>
@@ -5722,7 +5826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <f>Sheet1!$D69</f>
         <v>0</v>
@@ -5732,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <f>Sheet1!$D70</f>
         <v>0</v>
@@ -5742,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <f>Sheet1!$D71</f>
         <v>0</v>
@@ -5752,7 +5856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <f>Sheet1!$D72</f>
         <v>0</v>

</xml_diff>

<commit_message>
Issue on week, month averages
</commit_message>
<xml_diff>
--- a/HRV trend test data.xlsx
+++ b/HRV trend test data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcte\Non OneDrive Docs\GitHub\HRVApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8127537-8215-4E03-9C3A-39853D85F46E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E9BF16-4F5C-421D-B42A-942077EFAFA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5057" yWindow="1911" windowWidth="27009" windowHeight="16603" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5057" yWindow="1911" windowWidth="27009" windowHeight="16603" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="output" sheetId="2" r:id="rId2"/>
     <sheet name="More normal" sheetId="3" r:id="rId3"/>
+    <sheet name="21 days" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>Assume base date comes from app as today in UTC time. Data here is always an offset</t>
   </si>
@@ -3589,6 +3590,1154 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'21 days'!#REF!</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'21 days'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-83BE-4794-8154-3D0833D2974F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="11364207"/>
+        <c:axId val="11362127"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="11364207"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11362127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="11362127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11364207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'21 days'!#REF!</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'21 days'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'21 days'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BBE-4158-9960-F79D610588FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="280811871"/>
+        <c:axId val="280807711"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="280811871"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="280807711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="280807711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="280811871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'21 days'!$B$7:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'21 days'!$F$7:$F$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>64.282947348761965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.953083775466965</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.24570233820333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.923383916722713</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.671257449320464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.705846288932435</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4277072537491904E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.959261118872057</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.424146983461483</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>69.627538631818368</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57.994530955157614</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.511912664222514</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39.939200282095356</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66.825409938898858</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>64.451484468276377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-598B-4EA1-B854-70206ADE02D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1856839263"/>
+        <c:axId val="1856839679"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1856839263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1856839679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1856839679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1856839263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3789,6 +4938,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5854,6 +7123,1554 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6547,6 +9364,125 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>239485</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>149677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE183B0-C4C1-4AB4-84B8-1D0D5A027D81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>168651</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>8163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>482958</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>68994</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06F8D7A2-5B52-485D-953C-9AA02424D89A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>481425</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>406298</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>26215</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E72636A4-BEFF-45EA-A458-F717A85EBA15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6828,8 +9764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -8995,7 +11931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3E5EB3-BA15-47C5-9667-8B5EE7F07FA1}">
   <dimension ref="A4:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E61" sqref="D5:E61"/>
     </sheetView>
   </sheetViews>
@@ -12547,4 +15483,599 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298F89FB-98EE-4E33-98BE-E60621AA7FE2}">
+  <dimension ref="A1:L69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
+  <cols>
+    <col min="2" max="2" width="11.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <f>60*60*24</f>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <f>60*60</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="29.15">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D63" si="0">B7*$H$4+C7*$H$5</f>
+        <v>1821600</v>
+      </c>
+      <c r="E7" cm="1">
+        <f t="array" ref="E7">INDEX($L$7:$L$23,MOD(A7,17)+1,1)</f>
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <f>35*SIN(B7)+ 35</f>
+        <v>64.282947348761965</v>
+      </c>
+      <c r="L7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1735200</v>
+      </c>
+      <c r="E8" cm="1">
+        <f t="array" ref="E8">INDEX($L$7:$L$23,MOD(A8,17)+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F63" si="1">35*SIN(B8)+ 35</f>
+        <v>66.953083775466965</v>
+      </c>
+      <c r="L8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1648800</v>
+      </c>
+      <c r="E9" cm="1">
+        <f t="array" ref="E9">INDEX($L$7:$L$23,MOD(A9,17)+1,1)</f>
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>40.24570233820333</v>
+      </c>
+      <c r="L9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+      <c r="E10" cm="1">
+        <f t="array" ref="E10">INDEX($L$7:$L$23,MOD(A10,17)+1,1)</f>
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+      <c r="E11" cm="1">
+        <f t="array" ref="E11">INDEX($L$7:$L$23,MOD(A11,17)+1,1)</f>
+        <v>35</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1389600</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12">INDEX($L$7:$L$23,MOD(A12,17)+1,1)</f>
+        <v>38</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>24.923383916722713</v>
+      </c>
+      <c r="L12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="E13" cm="1">
+        <f t="array" ref="E13">INDEX($L$7:$L$23,MOD(A13,17)+1,1)</f>
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1220400</v>
+      </c>
+      <c r="E14" cm="1">
+        <f t="array" ref="E14">INDEX($L$7:$L$23,MOD(A14,17)+1,1)</f>
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>69.671257449320464</v>
+      </c>
+      <c r="L14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1137600</v>
+      </c>
+      <c r="E15" cm="1">
+        <f t="array" ref="E15">INDEX($L$7:$L$23,MOD(A15,17)+1,1)</f>
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>49.705846288932435</v>
+      </c>
+      <c r="L15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+      <c r="E16" cm="1">
+        <f t="array" ref="E16">INDEX($L$7:$L$23,MOD(A16,17)+1,1)</f>
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>957600</v>
+      </c>
+      <c r="E17" cm="1">
+        <f t="array" ref="E17">INDEX($L$7:$L$23,MOD(A17,17)+1,1)</f>
+        <v>17</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>3.4277072537491904E-4</v>
+      </c>
+      <c r="L17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>874800</v>
+      </c>
+      <c r="E18" cm="1">
+        <f t="array" ref="E18">INDEX($L$7:$L$23,MOD(A18,17)+1,1)</f>
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>15.959261118872057</v>
+      </c>
+      <c r="L18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>788400</v>
+      </c>
+      <c r="E19" cm="1">
+        <f t="array" ref="E19">INDEX($L$7:$L$23,MOD(A19,17)+1,1)</f>
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>49.424146983461483</v>
+      </c>
+      <c r="L19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>702000</v>
+      </c>
+      <c r="E20" cm="1">
+        <f t="array" ref="E20">INDEX($L$7:$L$23,MOD(A20,17)+1,1)</f>
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>69.627538631818368</v>
+      </c>
+      <c r="L20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>615600</v>
+      </c>
+      <c r="E21" cm="1">
+        <f t="array" ref="E21">INDEX($L$7:$L$23,MOD(A21,17)+1,1)</f>
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>57.994530955157614</v>
+      </c>
+      <c r="L21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>10800</v>
+      </c>
+      <c r="E22" cm="1">
+        <f t="array" ref="E22">INDEX($L$7:$L$23,MOD(A22,17)+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="L22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>10800</v>
+      </c>
+      <c r="E23" cm="1">
+        <f t="array" ref="E23">INDEX($L$7:$L$23,MOD(A23,17)+1,1)</f>
+        <v>19</v>
+      </c>
+      <c r="L23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>356400</v>
+      </c>
+      <c r="E24" cm="1">
+        <f t="array" ref="E24">INDEX($L$7:$L$23,MOD(A24,17)+1,1)</f>
+        <v>24</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>8.511912664222514</v>
+      </c>
+      <c r="L24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>270000</v>
+      </c>
+      <c r="E25" cm="1">
+        <f t="array" ref="E25">INDEX($L$7:$L$23,MOD(A25,17)+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>39.939200282095356</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>183600</v>
+      </c>
+      <c r="E26" cm="1">
+        <f t="array" ref="E26">INDEX($L$7:$L$23,MOD(A26,17)+1,1)</f>
+        <v>22</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>66.825409938898858</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>97200</v>
+      </c>
+      <c r="E27" cm="1">
+        <f t="array" ref="E27">INDEX($L$7:$L$23,MOD(A27,17)+1,1)</f>
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>64.451484468276377</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" ht="15.45">
+      <c r="I61" s="2"/>
+    </row>
+    <row r="69" spans="6:6" ht="15.45">
+      <c r="F69" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>